<commit_message>
Update to Entities 0.50
</commit_message>
<xml_diff>
--- a/Assets/Systems/IAUS/Curves.xlsx
+++ b/Assets/Systems/IAUS/Curves.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main Game Folder\ECS IAUS sytstem\Assets\Scripts\IAUS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Main Game Folder\ECS IAUS sytstem\Assets\Systems\IAUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -197,37 +197,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-3.427916099383399E-2</c:v>
+                  <c:v>2.8907629014118807E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.9666306624440715E-4</c:v>
+                  <c:v>1.2706188955274866E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5173773371015513E-2</c:v>
+                  <c:v>5.5663784569929264E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30640798364644595</c:v>
+                  <c:v>2.4035891025411371E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5935920163535543</c:v>
+                  <c:v>9.7763394186293651E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.80482622662898451</c:v>
+                  <c:v>0.32283458044648961</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.90049666306624443</c:v>
+                  <c:v>0.67716541955351006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9342791609938339</c:v>
+                  <c:v>0.90223660581370613</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.94512573721099469</c:v>
+                  <c:v>0.97596410897458874</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94850013331132521</c:v>
+                  <c:v>0.99443362154300707</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.9495395546737434</c:v>
+                  <c:v>0.9987293811044724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,37 +256,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.15080759462076365</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15256996150155389</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15814136789161803</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17542857018710889</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22610467385671573</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35291917331014278</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.57499999999999996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.79708082668985725</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.92389532614328429</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97457142981289102</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99185863210838199</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,37 +315,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.8992935212239328</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89770062259718264</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8925477276678736</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.87617181149515999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8269315552545109</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70050775077933258</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47499999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24949224922066743</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12306844474548922</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.3828188504839978E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.7452272332126395E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,37 +374,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.094061020536008E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2993249278280383E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9482299073766862E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9616805276750378E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.8639561315468915E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24634115479651919</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.505</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76365884520348082</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.91136043868453109</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97038319472324963</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99051770092623315</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,11 +420,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-882779408"/>
-        <c:axId val="-882791376"/>
+        <c:axId val="2127769232"/>
+        <c:axId val="2127763792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-882779408"/>
+        <c:axId val="2127769232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +467,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-882791376"/>
+        <c:crossAx val="2127763792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -475,7 +475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-882791376"/>
+        <c:axId val="2127763792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-882779408"/>
+        <c:crossAx val="2127769232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1464,7 +1464,7 @@
   <dimension ref="A2:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,16 +1478,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>40</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>40</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1497,30 +1488,12 @@
       <c r="C3">
         <v>-1</v>
       </c>
-      <c r="D3">
-        <v>-0.85</v>
-      </c>
-      <c r="E3">
-        <v>0.85</v>
-      </c>
-      <c r="F3">
-        <v>-0.99</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.95</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0.05</v>
-      </c>
-      <c r="F4">
         <v>1</v>
       </c>
     </row>
@@ -1529,16 +1502,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.35</v>
-      </c>
-      <c r="D5">
-        <v>0.6</v>
-      </c>
-      <c r="E5">
-        <v>0.6</v>
-      </c>
-      <c r="F5">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1575,19 +1539,19 @@
       </c>
       <c r="C12">
         <f>C$3*1/(1+POWER((1000*C$2*EXP(1)),($B12-C$5)))+C$4</f>
-        <v>-3.427916099383399E-2</v>
-      </c>
-      <c r="D12">
+        <v>2.8907629014118807E-4</v>
+      </c>
+      <c r="D12" t="e">
         <f t="shared" ref="D12:F27" si="0">D$3*1/(1+POWER((1000*D$2*EXP(1)),($B12-D$5)))+D$4</f>
-        <v>0.15080759462076365</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0.8992935212239328</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>1.094061020536008E-2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E12" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F12" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1601,19 +1565,19 @@
       </c>
       <c r="C13">
         <f t="shared" ref="C13:F28" si="1">C$3*1/(1+POWER((1000*C$2*EXP(1)),($B13-C$5)))+C$4</f>
-        <v>-4.9666306624440715E-4</v>
+        <v>1.2706188955274866E-3</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0.15256996150155389</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.89770062259718264</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>1.2993249278280383E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,19 +1591,19 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>9.5173773371015513E-2</v>
+        <v>5.5663784569929264E-3</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>0.15814136789161803</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0.8925477276678736</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>1.9482299073766862E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1653,19 +1617,19 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.30640798364644595</v>
+        <v>2.4035891025411371E-2</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>0.17542857018710889</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.87617181149515999</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>3.9616805276750378E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,19 +1643,19 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>0.5935920163535543</v>
+        <v>9.7763394186293651E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0.22610467385671573</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.8269315552545109</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>9.8639561315468915E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,19 +1669,19 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>0.80482622662898451</v>
+        <v>0.32283458044648961</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>0.35291917331014278</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0.70050775077933258</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0.24634115479651919</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1731,19 +1695,19 @@
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.90049666306624443</v>
+        <v>0.67716541955351006</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>0.57499999999999996</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>0.47499999999999998</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>0.505</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,19 +1721,19 @@
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>0.9342791609938339</v>
+        <v>0.90223660581370613</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0.79708082668985725</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>0.24949224922066743</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0.76365884520348082</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1783,19 +1747,19 @@
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>0.94512573721099469</v>
+        <v>0.97596410897458874</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>0.92389532614328429</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>0.12306844474548922</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>0.91136043868453109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1809,19 +1773,19 @@
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>0.94850013331132521</v>
+        <v>0.99443362154300707</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>0.97457142981289102</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>7.3828188504839978E-2</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>0.97038319472324963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1835,19 +1799,19 @@
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>0.9495395546737434</v>
+        <v>0.9987293811044724</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>0.99185863210838199</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>5.7452272332126395E-2</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>0.99051770092623315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1861,19 +1825,19 @@
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>0.949858749404763</v>
+        <v>0.99971092370985881</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>0.99743003849844614</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>5.2299377402817482E-2</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>0.99700675072171963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,19 +1851,19 @@
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>0.94995667821208785</v>
+        <v>0.9999342826496056</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>0.99919240537923626</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>5.0706478776067279E-2</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>0.99905938979463993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1913,19 +1877,19 @@
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>0.94998671403916057</v>
+        <v>0.99998506268115539</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>0.99974657976228698</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>5.021678189573632E-2</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>0.9997048399584284</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1939,19 +1903,19 @@
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>0.94999592553567169</v>
+        <v>0.99999660493404263</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>0.99992051325137576</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>5.0066492607181691E-2</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>0.99990742131630828</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,19 +1929,19 @@
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>0.94999875047399751</v>
+        <v>0.99999922835080568</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>0.99997507201566671</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>5.0020392499894789E-2</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>0.9999709662300118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1991,19 +1955,19 @@
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>0.94999961680553635</v>
+        <v>0.99999982461569836</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>0.99999218263377132</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>5.0006253904486257E-2</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>0.999990895067569</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2017,19 +1981,19 @@
       </c>
       <c r="C29">
         <f t="shared" ref="C29:F29" si="10">C$3*1/(1+POWER((1000*C$2*EXP(1)),($B29-C$5)))+C$4</f>
-        <v>0.94999988248511158</v>
+        <v>0.99999996013779402</v>
       </c>
       <c r="D29">
         <f t="shared" si="10"/>
-        <v>0.99999754852339739</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <f t="shared" si="10"/>
-        <v>5.0001917904644769E-2</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <f t="shared" si="10"/>
-        <v>0.9999971447507805</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start having NPC run from large threats areas
</commit_message>
<xml_diff>
--- a/Assets/Systems/IAUS/Curves.xlsx
+++ b/Assets/Systems/IAUS/Curves.xlsx
@@ -118,7 +118,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10344203849518811"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.89655796150481193"/>
+          <c:h val="0.73577136191309422"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -256,37 +266,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-1.1125000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-0.51250000000000018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-1.2500000000000178E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.38750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.6875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.88749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.98749999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.98750000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.88750000000000018</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.68750000000000022</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.38750000000000051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,11 +430,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2127769232"/>
-        <c:axId val="2127763792"/>
+        <c:axId val="202284640"/>
+        <c:axId val="202274848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127769232"/>
+        <c:axId val="202284640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127763792"/>
+        <c:crossAx val="202274848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -475,7 +485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127763792"/>
+        <c:axId val="202274848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +536,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127769232"/>
+        <c:crossAx val="202284640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1463,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,6 +1490,9 @@
       <c r="C2">
         <v>1000</v>
       </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1488,6 +1501,9 @@
       <c r="C3">
         <v>-1</v>
       </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1496,6 +1512,9 @@
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1504,6 +1523,9 @@
       <c r="C5">
         <v>0.55000000000000004</v>
       </c>
+      <c r="D5">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1541,12 +1563,12 @@
         <f>C$3*1/(1+POWER((1000*C$2*EXP(1)),($B12-C$5)))+C$4</f>
         <v>2.8907629014118807E-4</v>
       </c>
-      <c r="D12" t="e">
-        <f t="shared" ref="D12:F27" si="0">D$3*1/(1+POWER((1000*D$2*EXP(1)),($B12-D$5)))+D$4</f>
-        <v>#NUM!</v>
+      <c r="D12">
+        <f>1-($D$2*(A12-$D$5)^$D$3+$D$4)</f>
+        <v>-1.1125000000000003</v>
       </c>
       <c r="E12" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D12:F27" si="0">E$3*1/(1+POWER((1000*E$2*EXP(1)),($B12-E$5)))+E$4</f>
         <v>#NUM!</v>
       </c>
       <c r="F12" t="e">
@@ -1568,8 +1590,8 @@
         <v>1.2706188955274866E-3</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D13:D29" si="2">1-($D$2*(A13-$D$5)^$D$3+$D$4)</f>
+        <v>-0.51250000000000018</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -1582,11 +1604,11 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" ref="A14:B22" si="2">A13+0.1</f>
+        <f t="shared" ref="A14:B22" si="3">A13+0.1</f>
         <v>0.2</v>
       </c>
       <c r="B14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="C14">
@@ -1594,8 +1616,8 @@
         <v>5.5663784569929264E-3</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-1.2500000000000178E-2</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
@@ -1608,11 +1630,11 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="B15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="C15">
@@ -1620,8 +1642,8 @@
         <v>2.4035891025411371E-2</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.38750000000000007</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
@@ -1634,11 +1656,11 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="B16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
       <c r="C16">
@@ -1646,8 +1668,8 @@
         <v>9.7763394186293651E-2</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.6875</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -1660,11 +1682,11 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="B17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C17">
@@ -1672,8 +1694,8 @@
         <v>0.32283458044648961</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.88749999999999996</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
@@ -1686,11 +1708,11 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="B18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="C18">
@@ -1698,8 +1720,8 @@
         <v>0.67716541955351006</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.98749999999999993</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -1712,11 +1734,11 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
       <c r="C19">
@@ -1724,8 +1746,8 @@
         <v>0.90223660581370613</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.98750000000000004</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
@@ -1738,11 +1760,11 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="C20">
@@ -1750,8 +1772,8 @@
         <v>0.97596410897458874</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.88750000000000018</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
@@ -1764,11 +1786,11 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="B21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="C21">
@@ -1776,8 +1798,8 @@
         <v>0.99443362154300707</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.68750000000000022</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
@@ -1790,11 +1812,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="B22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="C22">
@@ -1802,8 +1824,8 @@
         <v>0.9987293811044724</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.38750000000000051</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
@@ -1816,11 +1838,11 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ref="A23:B23" si="3">A22+0.1</f>
+        <f t="shared" ref="A23:B23" si="4">A22+0.1</f>
         <v>1.0999999999999999</v>
       </c>
       <c r="B23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0999999999999999</v>
       </c>
       <c r="C23">
@@ -1828,8 +1850,8 @@
         <v>0.99971092370985881</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-1.2499999999999289E-2</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
@@ -1842,11 +1864,11 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" ref="A24:B24" si="4">A23+0.1</f>
+        <f t="shared" ref="A24:B24" si="5">A23+0.1</f>
         <v>1.2</v>
       </c>
       <c r="B24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2</v>
       </c>
       <c r="C24">
@@ -1854,8 +1876,8 @@
         <v>0.9999342826496056</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-0.51249999999999973</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
@@ -1868,11 +1890,11 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" ref="A25:B25" si="5">A24+0.1</f>
+        <f t="shared" ref="A25:B25" si="6">A24+0.1</f>
         <v>1.3</v>
       </c>
       <c r="B25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
       <c r="C25">
@@ -1880,8 +1902,8 @@
         <v>0.99998506268115539</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-1.1125000000000003</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
@@ -1894,11 +1916,11 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" ref="A26:B26" si="6">A25+0.1</f>
+        <f t="shared" ref="A26:B26" si="7">A25+0.1</f>
         <v>1.4000000000000001</v>
       </c>
       <c r="B26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="C26">
@@ -1906,8 +1928,8 @@
         <v>0.99999660493404263</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-1.8125000000000009</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
@@ -1920,11 +1942,11 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" ref="A27:B27" si="7">A26+0.1</f>
+        <f t="shared" ref="A27:B27" si="8">A26+0.1</f>
         <v>1.5000000000000002</v>
       </c>
       <c r="B27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5000000000000002</v>
       </c>
       <c r="C27">
@@ -1932,8 +1954,8 @@
         <v>0.99999922835080568</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-2.6125000000000016</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
@@ -1946,11 +1968,11 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" ref="A28:B28" si="8">A27+0.1</f>
+        <f t="shared" ref="A28:B28" si="9">A27+0.1</f>
         <v>1.6000000000000003</v>
       </c>
       <c r="B28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.6000000000000003</v>
       </c>
       <c r="C28">
@@ -1958,8 +1980,8 @@
         <v>0.99999982461569836</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-3.5125000000000028</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
@@ -1972,27 +1994,27 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" ref="A29:B29" si="9">A28+0.1</f>
+        <f t="shared" ref="A29:B29" si="10">A28+0.1</f>
         <v>1.7000000000000004</v>
       </c>
       <c r="B29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.7000000000000004</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:F29" si="10">C$3*1/(1+POWER((1000*C$2*EXP(1)),($B29-C$5)))+C$4</f>
+        <f t="shared" ref="C29:F29" si="11">C$3*1/(1+POWER((1000*C$2*EXP(1)),($B29-C$5)))+C$4</f>
         <v>0.99999996013779402</v>
       </c>
       <c r="D29">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-4.5125000000000028</v>
       </c>
       <c r="E29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>